<commit_message>
Refactor MqmsTimetracking and clickUpApi to support batch requests and improve time entry payload handling with assignee data
</commit_message>
<xml_diff>
--- a/public/IRAZU - Planilla Produccion - ANAIS ARCHILA.xlsx
+++ b/public/IRAZU - Planilla Produccion - ANAIS ARCHILA.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\IRAZU INC\HR\CONTRATISTAS\ANAIS ARCHILA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\93jad\Documents\apps\irazu-tools\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF36A24E-5C28-4475-B38D-316A86EE7BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3202A0C-9EF8-4506-9C09-9E8045A9D2CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iyddLnG9G1/BU6+UjMHcnLFNeR1swpOpdSatsqi52Xx3HCZdeGncXXaq7i20dCh+FuZ87JFti4SMDARXg5xrJg==" workbookSaltValue="fD9mHn+UnAEtooXlBbGP1Q==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3375" yWindow="3375" windowWidth="28800" windowHeight="15345" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="2" state="hidden" r:id="rId1"/>
@@ -237,14 +237,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
-    <numFmt numFmtId="167" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="168" formatCode="dd/mm/yy;@"/>
-    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="171" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="167" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -456,11 +456,11 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -476,13 +476,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,16 +499,16 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
@@ -519,18 +519,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -538,38 +538,41 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="14" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="12" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="16" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="16" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -578,46 +581,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="8">
-    <cellStyle name="Hipervínculo" xfId="7" builtinId="8"/>
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="3" builtinId="4"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Moneda 2" xfId="5" xr:uid="{3F787E62-6C98-4723-A2CB-8F3F7C8ABBBD}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{C5DCB0ED-A782-484C-8270-D44673E7F5BF}"/>
     <cellStyle name="Normal 3" xfId="6" xr:uid="{F3589114-3786-4C7E-8E05-0A5B3EE5C626}"/>
-    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -984,7 +959,7 @@
       <selection activeCell="D4" sqref="D4:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
@@ -1134,10 +1109,10 @@
   <dimension ref="A1:N596"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.42578125" style="6" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="6" customWidth="1"/>
@@ -1165,11 +1140,11 @@
       <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
@@ -1178,11 +1153,11 @@
       <c r="B2" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
     </row>
     <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
@@ -1279,8 +1254,8 @@
       <c r="K10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
+      <c r="M10" s="57"/>
+      <c r="N10" s="57"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
@@ -1312,8 +1287,8 @@
         <f>IFERROR(VLOOKUP(C11,Datos!#REF!,5,0),0)*D11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
@@ -1345,8 +1320,8 @@
         <f>IFERROR(VLOOKUP(C12,Datos!#REF!,5,0),0)*D12</f>
         <v>0</v>
       </c>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
@@ -1378,8 +1353,8 @@
         <f>IFERROR(VLOOKUP(C13,Datos!#REF!,5,0),0)*D13</f>
         <v>0</v>
       </c>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="57"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
@@ -1411,8 +1386,8 @@
         <f>IFERROR(VLOOKUP(C14,Datos!#REF!,5,0),0)*D14</f>
         <v>0</v>
       </c>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="57"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="str">
@@ -1444,8 +1419,8 @@
         <f>IFERROR(VLOOKUP(C15,Datos!#REF!,5,0),0)*D15</f>
         <v>0</v>
       </c>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="str">
@@ -1477,8 +1452,8 @@
         <f>IFERROR(VLOOKUP(C16,Datos!#REF!,5,0),0)*D16</f>
         <v>0</v>
       </c>
-      <c r="M16" s="59"/>
-      <c r="N16" s="59"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
@@ -1510,8 +1485,8 @@
         <f>IFERROR(VLOOKUP(C17,Datos!#REF!,5,0),0)*D17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
+      <c r="M17" s="57"/>
+      <c r="N17" s="57"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
@@ -1543,8 +1518,8 @@
         <f>IFERROR(VLOOKUP(C18,Datos!#REF!,5,0),0)*D18</f>
         <v>0</v>
       </c>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
+      <c r="M18" s="57"/>
+      <c r="N18" s="57"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="str">
@@ -14052,7 +14027,7 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
     <col min="2" max="2" width="61.7109375" customWidth="1"/>

</xml_diff>

<commit_message>
Update Excel Templates for vendors
</commit_message>
<xml_diff>
--- a/public/IRAZU - Planilla Produccion - ANAIS ARCHILA.xlsx
+++ b/public/IRAZU - Planilla Produccion - ANAIS ARCHILA.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Dropbox\IRAZU INC\HR\CONTRATISTAS\ANAIS ARCHILA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF36A24E-5C28-4475-B38D-316A86EE7BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="iyddLnG9G1/BU6+UjMHcnLFNeR1swpOpdSatsqi52Xx3HCZdeGncXXaq7i20dCh+FuZ87JFti4SMDARXg5xrJg==" workbookSaltValue="fD9mHn+UnAEtooXlBbGP1Q==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5951BA0D-6BF7-43EE-8052-391D1EF9C3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="vPcEjzACITSAbf9t1/w5A+sUVCQrqJbxF+0B/h3+rlS5NHenbhgUGZD7Fn5+7O4WzrZh3u0kpt6kIbcyPQPd+Q==" workbookSaltValue="rpQ+vNAUdkq0GlXjLFrzlg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="2" state="hidden" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>CANTIDAD</t>
   </si>
@@ -231,6 +231,15 @@
   <si>
     <t>csalazar@irazutechnology.com</t>
   </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>CCI - REDESIGN</t>
+  </si>
+  <si>
+    <t>REDESIGN (HR)</t>
+  </si>
 </sst>
 </file>
 
@@ -367,7 +376,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +422,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +479,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -526,9 +541,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,14 +584,27 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -592,32 +617,7 @@
     <cellStyle name="Normal 3" xfId="6" xr:uid="{F3589114-3786-4C7E-8E05-0A5B3EE5C626}"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -978,10 +978,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B1:L5"/>
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:F5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,63 +1065,95 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="37">
-        <f t="shared" ref="H4:H5" si="0">I4/$C$2</f>
+      <c r="H4" s="36">
+        <f t="shared" ref="H4:H6" si="0">I4/$C$2</f>
         <v>1.75E-4</v>
       </c>
-      <c r="I4" s="42">
+      <c r="I4" s="41">
         <v>70</v>
       </c>
-      <c r="J4" s="36">
+      <c r="J4" s="35">
         <v>21</v>
       </c>
-      <c r="K4" s="43">
+      <c r="K4" s="42">
         <f>+J4/I4</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="40">
         <f t="shared" si="0"/>
         <v>1.3750000000000001E-4</v>
       </c>
-      <c r="I5" s="42">
+      <c r="I5" s="41">
         <v>55</v>
       </c>
-      <c r="J5" s="44">
+      <c r="J5" s="43">
         <v>16.5</v>
       </c>
-      <c r="K5" s="43">
+      <c r="K5" s="42">
         <f>+J5/I5</f>
         <v>0.3</v>
       </c>
     </row>
+    <row r="6" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="40">
+        <f t="shared" si="0"/>
+        <v>8.7499999999999999E-5</v>
+      </c>
+      <c r="I6" s="41">
+        <v>35</v>
+      </c>
+      <c r="J6" s="43">
+        <f>+I6*0.3</f>
+        <v>10.5</v>
+      </c>
+      <c r="K6" s="42">
+        <f>+J6/I6</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="59"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QAKpTnHdW2bJpXb2tMFU0MyEL0haAfpsyvv+5Kbt9yaOZ4Z9ay7vNMHxRVoj7U1+sJxPNXa6AW7ARSj8LBllyg==" saltValue="5UwPPYUz/xR51+Jws4dlxw==" spinCount="100000" sheet="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <autoFilter ref="A3:N3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1133,8 +1165,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N596"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,9 +1191,10 @@
       <c r="A1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="61" t="s">
         <v>44</v>
       </c>
+      <c r="C1" s="62"/>
       <c r="D1" s="25" t="s">
         <v>35</v>
       </c>
@@ -1175,9 +1208,10 @@
       <c r="A2" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="61" t="s">
         <v>45</v>
       </c>
+      <c r="C2" s="62"/>
       <c r="E2" s="58" t="s">
         <v>37</v>
       </c>
@@ -1188,9 +1222,10 @@
       <c r="A3" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="33">
+      <c r="B3" s="61">
         <v>1127062933</v>
       </c>
+      <c r="C3" s="62"/>
       <c r="E3" s="30" t="s">
         <v>39</v>
       </c>
@@ -1201,9 +1236,10 @@
       <c r="A4" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="63" t="s">
         <v>46</v>
       </c>
+      <c r="C4" s="62"/>
       <c r="E4" s="26" t="s">
         <v>54</v>
       </c>
@@ -1220,7 +1256,7 @@
       <c r="A7" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="45"/>
+      <c r="B7" s="44"/>
       <c r="G7"/>
       <c r="K7"/>
     </row>
@@ -1279,8 +1315,8 @@
       <c r="K10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="56"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="str">
@@ -1297,8 +1333,8 @@
         <f>IFERROR(VLOOKUP(C11,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F11" s="46"/>
-      <c r="G11" s="46"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
       <c r="H11" s="1"/>
       <c r="I11" s="7">
         <f>IFERROR(VLOOKUP($C11,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1312,8 +1348,8 @@
         <f>IFERROR(VLOOKUP(C11,Datos!#REF!,5,0),0)*D11</f>
         <v>0</v>
       </c>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="56"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="str">
@@ -1330,8 +1366,8 @@
         <f>IFERROR(VLOOKUP(C12,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
       <c r="H12" s="1"/>
       <c r="I12" s="7">
         <f>IFERROR(VLOOKUP($C12,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1345,8 +1381,8 @@
         <f>IFERROR(VLOOKUP(C12,Datos!#REF!,5,0),0)*D12</f>
         <v>0</v>
       </c>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
+      <c r="M12" s="56"/>
+      <c r="N12" s="56"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
@@ -1363,8 +1399,8 @@
         <f>IFERROR(VLOOKUP(C13,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
       <c r="H13" s="1"/>
       <c r="I13" s="7">
         <f>IFERROR(VLOOKUP($C13,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1378,8 +1414,8 @@
         <f>IFERROR(VLOOKUP(C13,Datos!#REF!,5,0),0)*D13</f>
         <v>0</v>
       </c>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="str">
@@ -1396,8 +1432,8 @@
         <f>IFERROR(VLOOKUP(C14,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="46"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
       <c r="H14" s="1"/>
       <c r="I14" s="7">
         <f>IFERROR(VLOOKUP($C14,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1411,8 +1447,8 @@
         <f>IFERROR(VLOOKUP(C14,Datos!#REF!,5,0),0)*D14</f>
         <v>0</v>
       </c>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="str">
@@ -1429,8 +1465,8 @@
         <f>IFERROR(VLOOKUP(C15,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="1"/>
       <c r="I15" s="7">
         <f>IFERROR(VLOOKUP($C15,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1444,8 +1480,8 @@
         <f>IFERROR(VLOOKUP(C15,Datos!#REF!,5,0),0)*D15</f>
         <v>0</v>
       </c>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="str">
@@ -1462,8 +1498,8 @@
         <f>IFERROR(VLOOKUP(C16,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="1"/>
       <c r="I16" s="7">
         <f>IFERROR(VLOOKUP($C16,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1477,8 +1513,8 @@
         <f>IFERROR(VLOOKUP(C16,Datos!#REF!,5,0),0)*D16</f>
         <v>0</v>
       </c>
-      <c r="M16" s="59"/>
-      <c r="N16" s="59"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="str">
@@ -1495,8 +1531,8 @@
         <f>IFERROR(VLOOKUP(C17,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F17" s="46"/>
-      <c r="G17" s="47"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="1"/>
       <c r="I17" s="7">
         <f>IFERROR(VLOOKUP($C17,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1510,8 +1546,8 @@
         <f>IFERROR(VLOOKUP(C17,Datos!#REF!,5,0),0)*D17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="str">
@@ -1528,8 +1564,8 @@
         <f>IFERROR(VLOOKUP(C18,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F18" s="47"/>
-      <c r="G18" s="48"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
       <c r="H18" s="1"/>
       <c r="I18" s="7">
         <f>IFERROR(VLOOKUP($C18,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1543,8 +1579,8 @@
         <f>IFERROR(VLOOKUP(C18,Datos!#REF!,5,0),0)*D18</f>
         <v>0</v>
       </c>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="str">
@@ -1561,8 +1597,8 @@
         <f>IFERROR(VLOOKUP(C19,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="48"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="47"/>
       <c r="H19" s="1"/>
       <c r="I19" s="7">
         <f>IFERROR(VLOOKUP($C19,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1592,8 +1628,8 @@
         <f>IFERROR(VLOOKUP(C20,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="48"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="47"/>
       <c r="H20" s="1"/>
       <c r="I20" s="7">
         <f>IFERROR(VLOOKUP($C20,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1623,8 +1659,8 @@
         <f>IFERROR(VLOOKUP(C21,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="48"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="47"/>
       <c r="H21" s="1"/>
       <c r="I21" s="7">
         <f>IFERROR(VLOOKUP($C21,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1654,8 +1690,8 @@
         <f>IFERROR(VLOOKUP(C22,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="48"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="47"/>
       <c r="H22" s="1"/>
       <c r="I22" s="7">
         <f>IFERROR(VLOOKUP($C22,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1685,8 +1721,8 @@
         <f>IFERROR(VLOOKUP(C23,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="48"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="47"/>
       <c r="H23" s="1"/>
       <c r="I23" s="7">
         <f>IFERROR(VLOOKUP($C23,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1716,8 +1752,8 @@
         <f>IFERROR(VLOOKUP(C24,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="48"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="47"/>
       <c r="H24" s="1"/>
       <c r="I24" s="7">
         <f>IFERROR(VLOOKUP($C24,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1742,14 +1778,14 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="49"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="2" t="str">
         <f>IFERROR(VLOOKUP(C25,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="56"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="55"/>
       <c r="I25" s="7">
         <f>IFERROR(VLOOKUP($C25,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
@@ -1773,14 +1809,14 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="49"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="2" t="str">
         <f>IFERROR(VLOOKUP(C26,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F26" s="50"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="56"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="55"/>
       <c r="I26" s="7">
         <f>IFERROR(VLOOKUP($C26,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
@@ -1810,8 +1846,8 @@
         <f>IFERROR(VLOOKUP(C27,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
       <c r="H27" s="1"/>
       <c r="I27" s="7">
         <f>IFERROR(VLOOKUP($C27,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1825,7 +1861,7 @@
         <f>IFERROR(VLOOKUP(C27,Datos!#REF!,5,0),0)*D27</f>
         <v>0</v>
       </c>
-      <c r="N27" s="51"/>
+      <c r="N27" s="50"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="str">
@@ -1842,8 +1878,8 @@
         <f>IFERROR(VLOOKUP(C28,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F28" s="46"/>
-      <c r="G28" s="46"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
       <c r="H28" s="1"/>
       <c r="I28" s="7">
         <f>IFERROR(VLOOKUP($C28,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1873,8 +1909,8 @@
         <f>IFERROR(VLOOKUP(C29,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
       <c r="H29" s="1"/>
       <c r="I29" s="7">
         <f>IFERROR(VLOOKUP($C29,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1904,8 +1940,8 @@
         <f>IFERROR(VLOOKUP(C30,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
       <c r="H30" s="1"/>
       <c r="I30" s="7">
         <f>IFERROR(VLOOKUP($C30,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1935,8 +1971,8 @@
         <f>IFERROR(VLOOKUP(C31,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F31" s="55"/>
-      <c r="G31" s="48"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="47"/>
       <c r="H31" s="1"/>
       <c r="I31" s="7">
         <f>IFERROR(VLOOKUP($C31,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1966,8 +2002,8 @@
         <f>IFERROR(VLOOKUP(C32,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F32" s="55"/>
-      <c r="G32" s="48"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="47"/>
       <c r="H32" s="1"/>
       <c r="I32" s="7">
         <f>IFERROR(VLOOKUP($C32,Datos!$D$4:$J$39,7,0),0)</f>
@@ -1997,8 +2033,8 @@
         <f>IFERROR(VLOOKUP(C33,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F33" s="55"/>
-      <c r="G33" s="48"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="47"/>
       <c r="H33" s="1"/>
       <c r="I33" s="7">
         <f>IFERROR(VLOOKUP($C33,Datos!$D$4:$J$39,7,0),0)</f>
@@ -2028,18 +2064,18 @@
         <f>IFERROR(VLOOKUP(C34,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F34" s="55"/>
-      <c r="G34" s="48"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="47"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="52">
+      <c r="I34" s="51">
         <f>IFERROR(VLOOKUP($C34,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J34" s="53">
+      <c r="J34" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K34" s="54">
+      <c r="K34" s="53">
         <f>IFERROR(VLOOKUP(C34,Datos!#REF!,5,0),0)*D34</f>
         <v>0</v>
       </c>
@@ -2059,18 +2095,18 @@
         <f>IFERROR(VLOOKUP(C35,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F35" s="55"/>
-      <c r="G35" s="48"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="47"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="52">
+      <c r="I35" s="51">
         <f>IFERROR(VLOOKUP($C35,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J35" s="53">
+      <c r="J35" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K35" s="54">
+      <c r="K35" s="53">
         <f>IFERROR(VLOOKUP(C35,Datos!#REF!,5,0),0)*D35</f>
         <v>0</v>
       </c>
@@ -2090,18 +2126,18 @@
         <f>IFERROR(VLOOKUP(C36,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F36" s="55"/>
-      <c r="G36" s="48"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="47"/>
       <c r="H36" s="1"/>
-      <c r="I36" s="52">
+      <c r="I36" s="51">
         <f>IFERROR(VLOOKUP($C36,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J36" s="53">
+      <c r="J36" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K36" s="54">
+      <c r="K36" s="53">
         <f>IFERROR(VLOOKUP(C36,Datos!#REF!,5,0),0)*D36</f>
         <v>0</v>
       </c>
@@ -2121,18 +2157,18 @@
         <f>IFERROR(VLOOKUP(C37,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F37" s="55"/>
-      <c r="G37" s="48"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="47"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="52">
+      <c r="I37" s="51">
         <f>IFERROR(VLOOKUP($C37,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J37" s="53">
+      <c r="J37" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K37" s="54">
+      <c r="K37" s="53">
         <f>IFERROR(VLOOKUP(C37,Datos!#REF!,5,0),0)*D37</f>
         <v>0</v>
       </c>
@@ -2152,18 +2188,18 @@
         <f>IFERROR(VLOOKUP(C38,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F38" s="55"/>
-      <c r="G38" s="48"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="47"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="52">
+      <c r="I38" s="51">
         <f>IFERROR(VLOOKUP($C38,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J38" s="53">
+      <c r="J38" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K38" s="54">
+      <c r="K38" s="53">
         <f>IFERROR(VLOOKUP(C38,Datos!#REF!,5,0),0)*D38</f>
         <v>0</v>
       </c>
@@ -2183,18 +2219,18 @@
         <f>IFERROR(VLOOKUP(C39,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F39" s="55"/>
-      <c r="G39" s="48"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="47"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="52">
+      <c r="I39" s="51">
         <f>IFERROR(VLOOKUP($C39,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J39" s="53">
+      <c r="J39" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K39" s="54">
+      <c r="K39" s="53">
         <f>IFERROR(VLOOKUP(C39,Datos!#REF!,5,0),0)*D39</f>
         <v>0</v>
       </c>
@@ -2214,18 +2250,18 @@
         <f>IFERROR(VLOOKUP(C40,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F40" s="55"/>
-      <c r="G40" s="48"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="47"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="52">
+      <c r="I40" s="51">
         <f>IFERROR(VLOOKUP($C40,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J40" s="53">
+      <c r="J40" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K40" s="54">
+      <c r="K40" s="53">
         <f>IFERROR(VLOOKUP(C40,Datos!#REF!,5,0),0)*D40</f>
         <v>0</v>
       </c>
@@ -2245,18 +2281,18 @@
         <f>IFERROR(VLOOKUP(C41,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F41" s="55"/>
-      <c r="G41" s="48"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="47"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="52">
+      <c r="I41" s="51">
         <f>IFERROR(VLOOKUP($C41,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J41" s="53">
+      <c r="J41" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K41" s="54">
+      <c r="K41" s="53">
         <f>IFERROR(VLOOKUP(C41,Datos!#REF!,5,0),0)*D41</f>
         <v>0</v>
       </c>
@@ -2276,18 +2312,18 @@
         <f>IFERROR(VLOOKUP(C42,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F42" s="55"/>
-      <c r="G42" s="48"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="47"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="52">
+      <c r="I42" s="51">
         <f>IFERROR(VLOOKUP($C42,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J42" s="53">
+      <c r="J42" s="52">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K42" s="54">
+      <c r="K42" s="53">
         <f>IFERROR(VLOOKUP(C42,Datos!#REF!,5,0),0)*D42</f>
         <v>0</v>
       </c>
@@ -2307,18 +2343,18 @@
         <f>IFERROR(VLOOKUP(C43,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F43" s="55"/>
-      <c r="G43" s="48"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="47"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="52">
+      <c r="I43" s="51">
         <f>IFERROR(VLOOKUP($C43,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J43" s="53">
+      <c r="J43" s="52">
         <f t="shared" ref="J43:J74" si="1">IFERROR((+I43*D43),0)</f>
         <v>0</v>
       </c>
-      <c r="K43" s="54">
+      <c r="K43" s="53">
         <f>IFERROR(VLOOKUP(C43,Datos!#REF!,5,0),0)*D43</f>
         <v>0</v>
       </c>
@@ -2338,18 +2374,18 @@
         <f>IFERROR(VLOOKUP(C44,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F44" s="55"/>
-      <c r="G44" s="48"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="47"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="52">
+      <c r="I44" s="51">
         <f>IFERROR(VLOOKUP($C44,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J44" s="53">
+      <c r="J44" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K44" s="54">
+      <c r="K44" s="53">
         <f>IFERROR(VLOOKUP(C44,Datos!#REF!,5,0),0)*D44</f>
         <v>0</v>
       </c>
@@ -2369,18 +2405,18 @@
         <f>IFERROR(VLOOKUP(C45,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F45" s="55"/>
-      <c r="G45" s="48"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="47"/>
       <c r="H45" s="1"/>
-      <c r="I45" s="52">
+      <c r="I45" s="51">
         <f>IFERROR(VLOOKUP($C45,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J45" s="53">
+      <c r="J45" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K45" s="54">
+      <c r="K45" s="53">
         <f>IFERROR(VLOOKUP(C45,Datos!#REF!,5,0),0)*D45</f>
         <v>0</v>
       </c>
@@ -2400,18 +2436,18 @@
         <f>IFERROR(VLOOKUP(C46,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F46" s="55"/>
-      <c r="G46" s="48"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="47"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="52">
+      <c r="I46" s="51">
         <f>IFERROR(VLOOKUP($C46,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J46" s="53">
+      <c r="J46" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K46" s="54">
+      <c r="K46" s="53">
         <f>IFERROR(VLOOKUP(C46,Datos!#REF!,5,0),0)*D46</f>
         <v>0</v>
       </c>
@@ -2431,18 +2467,18 @@
         <f>IFERROR(VLOOKUP(C47,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F47" s="55"/>
-      <c r="G47" s="48"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="47"/>
       <c r="H47" s="1"/>
-      <c r="I47" s="52">
+      <c r="I47" s="51">
         <f>IFERROR(VLOOKUP($C47,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J47" s="53">
+      <c r="J47" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K47" s="54">
+      <c r="K47" s="53">
         <f>IFERROR(VLOOKUP(C47,Datos!#REF!,5,0),0)*D47</f>
         <v>0</v>
       </c>
@@ -2462,18 +2498,18 @@
         <f>IFERROR(VLOOKUP(C48,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F48" s="55"/>
-      <c r="G48" s="48"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="47"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="52">
+      <c r="I48" s="51">
         <f>IFERROR(VLOOKUP($C48,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J48" s="53">
+      <c r="J48" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K48" s="54">
+      <c r="K48" s="53">
         <f>IFERROR(VLOOKUP(C48,Datos!#REF!,5,0),0)*D48</f>
         <v>0</v>
       </c>
@@ -2493,18 +2529,18 @@
         <f>IFERROR(VLOOKUP(C49,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F49" s="55"/>
-      <c r="G49" s="48"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="47"/>
       <c r="H49" s="1"/>
-      <c r="I49" s="52">
+      <c r="I49" s="51">
         <f>IFERROR(VLOOKUP($C49,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J49" s="53">
+      <c r="J49" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K49" s="54">
+      <c r="K49" s="53">
         <f>IFERROR(VLOOKUP(C49,Datos!#REF!,5,0),0)*D49</f>
         <v>0</v>
       </c>
@@ -2524,18 +2560,18 @@
         <f>IFERROR(VLOOKUP(C50,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F50" s="55"/>
-      <c r="G50" s="48"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="47"/>
       <c r="H50" s="1"/>
-      <c r="I50" s="52">
+      <c r="I50" s="51">
         <f>IFERROR(VLOOKUP($C50,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J50" s="53">
+      <c r="J50" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K50" s="54">
+      <c r="K50" s="53">
         <f>IFERROR(VLOOKUP(C50,Datos!#REF!,5,0),0)*D50</f>
         <v>0</v>
       </c>
@@ -2555,18 +2591,18 @@
         <f>IFERROR(VLOOKUP(C51,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F51" s="55"/>
-      <c r="G51" s="48"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="47"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="52">
+      <c r="I51" s="51">
         <f>IFERROR(VLOOKUP($C51,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J51" s="53">
+      <c r="J51" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K51" s="54">
+      <c r="K51" s="53">
         <f>IFERROR(VLOOKUP(C51,Datos!#REF!,5,0),0)*D51</f>
         <v>0</v>
       </c>
@@ -2586,18 +2622,18 @@
         <f>IFERROR(VLOOKUP(C52,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F52" s="55"/>
-      <c r="G52" s="48"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="47"/>
       <c r="H52" s="1"/>
-      <c r="I52" s="52">
+      <c r="I52" s="51">
         <f>IFERROR(VLOOKUP($C52,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J52" s="53">
+      <c r="J52" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K52" s="54">
+      <c r="K52" s="53">
         <f>IFERROR(VLOOKUP(C52,Datos!#REF!,5,0),0)*D52</f>
         <v>0</v>
       </c>
@@ -2617,18 +2653,18 @@
         <f>IFERROR(VLOOKUP(C53,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F53" s="55"/>
-      <c r="G53" s="48"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="47"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="52">
+      <c r="I53" s="51">
         <f>IFERROR(VLOOKUP($C53,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J53" s="53">
+      <c r="J53" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K53" s="54">
+      <c r="K53" s="53">
         <f>IFERROR(VLOOKUP(C53,Datos!#REF!,5,0),0)*D53</f>
         <v>0</v>
       </c>
@@ -2648,18 +2684,18 @@
         <f>IFERROR(VLOOKUP(C54,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F54" s="55"/>
-      <c r="G54" s="48"/>
+      <c r="F54" s="54"/>
+      <c r="G54" s="47"/>
       <c r="H54" s="1"/>
-      <c r="I54" s="52">
+      <c r="I54" s="51">
         <f>IFERROR(VLOOKUP($C54,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J54" s="53">
+      <c r="J54" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K54" s="54">
+      <c r="K54" s="53">
         <f>IFERROR(VLOOKUP(C54,Datos!#REF!,5,0),0)*D54</f>
         <v>0</v>
       </c>
@@ -2679,18 +2715,18 @@
         <f>IFERROR(VLOOKUP(C55,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F55" s="55"/>
-      <c r="G55" s="48"/>
+      <c r="F55" s="54"/>
+      <c r="G55" s="47"/>
       <c r="H55" s="1"/>
-      <c r="I55" s="52">
+      <c r="I55" s="51">
         <f>IFERROR(VLOOKUP($C55,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J55" s="53">
+      <c r="J55" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K55" s="54">
+      <c r="K55" s="53">
         <f>IFERROR(VLOOKUP(C55,Datos!#REF!,5,0),0)*D55</f>
         <v>0</v>
       </c>
@@ -2710,18 +2746,18 @@
         <f>IFERROR(VLOOKUP(C56,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F56" s="55"/>
-      <c r="G56" s="48"/>
+      <c r="F56" s="54"/>
+      <c r="G56" s="47"/>
       <c r="H56" s="1"/>
-      <c r="I56" s="52">
+      <c r="I56" s="51">
         <f>IFERROR(VLOOKUP($C56,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J56" s="53">
+      <c r="J56" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K56" s="54">
+      <c r="K56" s="53">
         <f>IFERROR(VLOOKUP(C56,Datos!#REF!,5,0),0)*D56</f>
         <v>0</v>
       </c>
@@ -2741,18 +2777,18 @@
         <f>IFERROR(VLOOKUP(C57,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F57" s="55"/>
-      <c r="G57" s="48"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="47"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="52">
+      <c r="I57" s="51">
         <f>IFERROR(VLOOKUP($C57,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J57" s="53">
+      <c r="J57" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K57" s="54">
+      <c r="K57" s="53">
         <f>IFERROR(VLOOKUP(C57,Datos!#REF!,5,0),0)*D57</f>
         <v>0</v>
       </c>
@@ -2772,18 +2808,18 @@
         <f>IFERROR(VLOOKUP(C58,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F58" s="55"/>
-      <c r="G58" s="48"/>
+      <c r="F58" s="54"/>
+      <c r="G58" s="47"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="52">
+      <c r="I58" s="51">
         <f>IFERROR(VLOOKUP($C58,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J58" s="53">
+      <c r="J58" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K58" s="54">
+      <c r="K58" s="53">
         <f>IFERROR(VLOOKUP(C58,Datos!#REF!,5,0),0)*D58</f>
         <v>0</v>
       </c>
@@ -2803,18 +2839,18 @@
         <f>IFERROR(VLOOKUP(C59,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F59" s="55"/>
-      <c r="G59" s="48"/>
+      <c r="F59" s="54"/>
+      <c r="G59" s="47"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="52">
+      <c r="I59" s="51">
         <f>IFERROR(VLOOKUP($C59,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J59" s="53">
+      <c r="J59" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K59" s="54">
+      <c r="K59" s="53">
         <f>IFERROR(VLOOKUP(C59,Datos!#REF!,5,0),0)*D59</f>
         <v>0</v>
       </c>
@@ -2834,18 +2870,18 @@
         <f>IFERROR(VLOOKUP(C60,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F60" s="55"/>
-      <c r="G60" s="48"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="47"/>
       <c r="H60" s="1"/>
-      <c r="I60" s="52">
+      <c r="I60" s="51">
         <f>IFERROR(VLOOKUP($C60,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J60" s="53">
+      <c r="J60" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K60" s="54">
+      <c r="K60" s="53">
         <f>IFERROR(VLOOKUP(C60,Datos!#REF!,5,0),0)*D60</f>
         <v>0</v>
       </c>
@@ -2865,18 +2901,18 @@
         <f>IFERROR(VLOOKUP(C61,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F61" s="55"/>
-      <c r="G61" s="48"/>
+      <c r="F61" s="54"/>
+      <c r="G61" s="47"/>
       <c r="H61" s="1"/>
-      <c r="I61" s="52">
+      <c r="I61" s="51">
         <f>IFERROR(VLOOKUP($C61,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J61" s="53">
+      <c r="J61" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K61" s="54">
+      <c r="K61" s="53">
         <f>IFERROR(VLOOKUP(C61,Datos!#REF!,5,0),0)*D61</f>
         <v>0</v>
       </c>
@@ -2896,18 +2932,18 @@
         <f>IFERROR(VLOOKUP(C62,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F62" s="55"/>
-      <c r="G62" s="48"/>
+      <c r="F62" s="54"/>
+      <c r="G62" s="47"/>
       <c r="H62" s="1"/>
-      <c r="I62" s="52">
+      <c r="I62" s="51">
         <f>IFERROR(VLOOKUP($C62,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J62" s="53">
+      <c r="J62" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K62" s="54">
+      <c r="K62" s="53">
         <f>IFERROR(VLOOKUP(C62,Datos!#REF!,5,0),0)*D62</f>
         <v>0</v>
       </c>
@@ -2927,18 +2963,18 @@
         <f>IFERROR(VLOOKUP(C63,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F63" s="55"/>
-      <c r="G63" s="48"/>
+      <c r="F63" s="54"/>
+      <c r="G63" s="47"/>
       <c r="H63" s="1"/>
-      <c r="I63" s="52">
+      <c r="I63" s="51">
         <f>IFERROR(VLOOKUP($C63,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J63" s="53">
+      <c r="J63" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K63" s="54">
+      <c r="K63" s="53">
         <f>IFERROR(VLOOKUP(C63,Datos!#REF!,5,0),0)*D63</f>
         <v>0</v>
       </c>
@@ -2958,18 +2994,18 @@
         <f>IFERROR(VLOOKUP(C64,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F64" s="55"/>
-      <c r="G64" s="48"/>
+      <c r="F64" s="54"/>
+      <c r="G64" s="47"/>
       <c r="H64" s="1"/>
-      <c r="I64" s="52">
+      <c r="I64" s="51">
         <f>IFERROR(VLOOKUP($C64,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J64" s="53">
+      <c r="J64" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K64" s="54">
+      <c r="K64" s="53">
         <f>IFERROR(VLOOKUP(C64,Datos!#REF!,5,0),0)*D64</f>
         <v>0</v>
       </c>
@@ -2989,18 +3025,18 @@
         <f>IFERROR(VLOOKUP(C65,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F65" s="55"/>
-      <c r="G65" s="48"/>
+      <c r="F65" s="54"/>
+      <c r="G65" s="47"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="52">
+      <c r="I65" s="51">
         <f>IFERROR(VLOOKUP($C65,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J65" s="53">
+      <c r="J65" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K65" s="54">
+      <c r="K65" s="53">
         <f>IFERROR(VLOOKUP(C65,Datos!#REF!,5,0),0)*D65</f>
         <v>0</v>
       </c>
@@ -3020,18 +3056,18 @@
         <f>IFERROR(VLOOKUP(C66,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F66" s="55"/>
-      <c r="G66" s="48"/>
+      <c r="F66" s="54"/>
+      <c r="G66" s="47"/>
       <c r="H66" s="1"/>
-      <c r="I66" s="52">
+      <c r="I66" s="51">
         <f>IFERROR(VLOOKUP($C66,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J66" s="53">
+      <c r="J66" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K66" s="54">
+      <c r="K66" s="53">
         <f>IFERROR(VLOOKUP(C66,Datos!#REF!,5,0),0)*D66</f>
         <v>0</v>
       </c>
@@ -3051,18 +3087,18 @@
         <f>IFERROR(VLOOKUP(C67,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F67" s="55"/>
-      <c r="G67" s="48"/>
+      <c r="F67" s="54"/>
+      <c r="G67" s="47"/>
       <c r="H67" s="1"/>
-      <c r="I67" s="52">
+      <c r="I67" s="51">
         <f>IFERROR(VLOOKUP($C67,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J67" s="53">
+      <c r="J67" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K67" s="54">
+      <c r="K67" s="53">
         <f>IFERROR(VLOOKUP(C67,Datos!#REF!,5,0),0)*D67</f>
         <v>0</v>
       </c>
@@ -3082,18 +3118,18 @@
         <f>IFERROR(VLOOKUP(C68,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F68" s="55"/>
-      <c r="G68" s="48"/>
+      <c r="F68" s="54"/>
+      <c r="G68" s="47"/>
       <c r="H68" s="1"/>
-      <c r="I68" s="52">
+      <c r="I68" s="51">
         <f>IFERROR(VLOOKUP($C68,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J68" s="53">
+      <c r="J68" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K68" s="54">
+      <c r="K68" s="53">
         <f>IFERROR(VLOOKUP(C68,Datos!#REF!,5,0),0)*D68</f>
         <v>0</v>
       </c>
@@ -3113,18 +3149,18 @@
         <f>IFERROR(VLOOKUP(C69,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F69" s="55"/>
-      <c r="G69" s="48"/>
+      <c r="F69" s="54"/>
+      <c r="G69" s="47"/>
       <c r="H69" s="1"/>
-      <c r="I69" s="52">
+      <c r="I69" s="51">
         <f>IFERROR(VLOOKUP($C69,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J69" s="53">
+      <c r="J69" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K69" s="54">
+      <c r="K69" s="53">
         <f>IFERROR(VLOOKUP(C69,Datos!#REF!,5,0),0)*D69</f>
         <v>0</v>
       </c>
@@ -3144,18 +3180,18 @@
         <f>IFERROR(VLOOKUP(C70,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F70" s="55"/>
-      <c r="G70" s="48"/>
+      <c r="F70" s="54"/>
+      <c r="G70" s="47"/>
       <c r="H70" s="1"/>
-      <c r="I70" s="52">
+      <c r="I70" s="51">
         <f>IFERROR(VLOOKUP($C70,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J70" s="53">
+      <c r="J70" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K70" s="54">
+      <c r="K70" s="53">
         <f>IFERROR(VLOOKUP(C70,Datos!#REF!,5,0),0)*D70</f>
         <v>0</v>
       </c>
@@ -3175,18 +3211,18 @@
         <f>IFERROR(VLOOKUP(C71,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F71" s="55"/>
-      <c r="G71" s="48"/>
+      <c r="F71" s="54"/>
+      <c r="G71" s="47"/>
       <c r="H71" s="1"/>
-      <c r="I71" s="52">
+      <c r="I71" s="51">
         <f>IFERROR(VLOOKUP($C71,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J71" s="53">
+      <c r="J71" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K71" s="54">
+      <c r="K71" s="53">
         <f>IFERROR(VLOOKUP(C71,Datos!#REF!,5,0),0)*D71</f>
         <v>0</v>
       </c>
@@ -3206,18 +3242,18 @@
         <f>IFERROR(VLOOKUP(C72,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F72" s="55"/>
-      <c r="G72" s="48"/>
+      <c r="F72" s="54"/>
+      <c r="G72" s="47"/>
       <c r="H72" s="1"/>
-      <c r="I72" s="52">
+      <c r="I72" s="51">
         <f>IFERROR(VLOOKUP($C72,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J72" s="53">
+      <c r="J72" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K72" s="54">
+      <c r="K72" s="53">
         <f>IFERROR(VLOOKUP(C72,Datos!#REF!,5,0),0)*D72</f>
         <v>0</v>
       </c>
@@ -3237,18 +3273,18 @@
         <f>IFERROR(VLOOKUP(C73,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F73" s="55"/>
-      <c r="G73" s="48"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="47"/>
       <c r="H73" s="1"/>
-      <c r="I73" s="52">
+      <c r="I73" s="51">
         <f>IFERROR(VLOOKUP($C73,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J73" s="53">
+      <c r="J73" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K73" s="54">
+      <c r="K73" s="53">
         <f>IFERROR(VLOOKUP(C73,Datos!#REF!,5,0),0)*D73</f>
         <v>0</v>
       </c>
@@ -3268,18 +3304,18 @@
         <f>IFERROR(VLOOKUP(C74,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F74" s="55"/>
-      <c r="G74" s="48"/>
+      <c r="F74" s="54"/>
+      <c r="G74" s="47"/>
       <c r="H74" s="1"/>
-      <c r="I74" s="52">
+      <c r="I74" s="51">
         <f>IFERROR(VLOOKUP($C74,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J74" s="53">
+      <c r="J74" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K74" s="54">
+      <c r="K74" s="53">
         <f>IFERROR(VLOOKUP(C74,Datos!#REF!,5,0),0)*D74</f>
         <v>0</v>
       </c>
@@ -3299,18 +3335,18 @@
         <f>IFERROR(VLOOKUP(C75,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F75" s="55"/>
-      <c r="G75" s="48"/>
+      <c r="F75" s="54"/>
+      <c r="G75" s="47"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="52">
+      <c r="I75" s="51">
         <f>IFERROR(VLOOKUP($C75,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J75" s="53">
+      <c r="J75" s="52">
         <f t="shared" ref="J75:J106" si="2">IFERROR((+I75*D75),0)</f>
         <v>0</v>
       </c>
-      <c r="K75" s="54">
+      <c r="K75" s="53">
         <f>IFERROR(VLOOKUP(C75,Datos!#REF!,5,0),0)*D75</f>
         <v>0</v>
       </c>
@@ -3330,18 +3366,18 @@
         <f>IFERROR(VLOOKUP(C76,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F76" s="55"/>
-      <c r="G76" s="48"/>
+      <c r="F76" s="54"/>
+      <c r="G76" s="47"/>
       <c r="H76" s="1"/>
-      <c r="I76" s="52">
+      <c r="I76" s="51">
         <f>IFERROR(VLOOKUP($C76,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J76" s="53">
+      <c r="J76" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K76" s="54">
+      <c r="K76" s="53">
         <f>IFERROR(VLOOKUP(C76,Datos!#REF!,5,0),0)*D76</f>
         <v>0</v>
       </c>
@@ -3361,18 +3397,18 @@
         <f>IFERROR(VLOOKUP(C77,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F77" s="55"/>
-      <c r="G77" s="48"/>
+      <c r="F77" s="54"/>
+      <c r="G77" s="47"/>
       <c r="H77" s="1"/>
-      <c r="I77" s="52">
+      <c r="I77" s="51">
         <f>IFERROR(VLOOKUP($C77,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J77" s="53">
+      <c r="J77" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K77" s="54">
+      <c r="K77" s="53">
         <f>IFERROR(VLOOKUP(C77,Datos!#REF!,5,0),0)*D77</f>
         <v>0</v>
       </c>
@@ -3392,18 +3428,18 @@
         <f>IFERROR(VLOOKUP(C78,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F78" s="55"/>
-      <c r="G78" s="48"/>
+      <c r="F78" s="54"/>
+      <c r="G78" s="47"/>
       <c r="H78" s="1"/>
-      <c r="I78" s="52">
+      <c r="I78" s="51">
         <f>IFERROR(VLOOKUP($C78,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J78" s="53">
+      <c r="J78" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K78" s="54">
+      <c r="K78" s="53">
         <f>IFERROR(VLOOKUP(C78,Datos!#REF!,5,0),0)*D78</f>
         <v>0</v>
       </c>
@@ -3423,18 +3459,18 @@
         <f>IFERROR(VLOOKUP(C79,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F79" s="55"/>
-      <c r="G79" s="48"/>
+      <c r="F79" s="54"/>
+      <c r="G79" s="47"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="52">
+      <c r="I79" s="51">
         <f>IFERROR(VLOOKUP($C79,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J79" s="53">
+      <c r="J79" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K79" s="54">
+      <c r="K79" s="53">
         <f>IFERROR(VLOOKUP(C79,Datos!#REF!,5,0),0)*D79</f>
         <v>0</v>
       </c>
@@ -3454,18 +3490,18 @@
         <f>IFERROR(VLOOKUP(C80,Datos!$D$4:$I$39,4,0)," ")</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F80" s="55"/>
-      <c r="G80" s="48"/>
+      <c r="F80" s="54"/>
+      <c r="G80" s="47"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="52">
+      <c r="I80" s="51">
         <f>IFERROR(VLOOKUP($C80,Datos!$D$4:$J$39,7,0),0)</f>
         <v>0</v>
       </c>
-      <c r="J80" s="53">
+      <c r="J80" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K80" s="54">
+      <c r="K80" s="53">
         <f>IFERROR(VLOOKUP(C80,Datos!#REF!,5,0),0)*D80</f>
         <v>0</v>
       </c>
@@ -3531,7 +3567,7 @@
         <f>IFERROR(VLOOKUP(C82,Datos!#REF!,5,0),0)*D82</f>
         <v>0</v>
       </c>
-      <c r="M82" s="51"/>
+      <c r="M82" s="50"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="str">
@@ -13980,6 +14016,7 @@
       <c r="K595" s="5"/>
     </row>
     <row r="596" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C596" s="2"/>
       <c r="I596" s="7">
         <f>IFERROR(VLOOKUP($C596,Datos!$D$4:$J$4,7,0),0)</f>
         <v>0</v>
@@ -14012,7 +14049,7 @@
   <legacyDrawing r:id="rId5"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Datos!#REF!</xm:f>
@@ -14029,13 +14066,19 @@
           <x14:formula1>
             <xm:f>Referencias!$A$12:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C109:C709</xm:sqref>
+          <xm:sqref>C597:C709</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ACF9AC47-BDEC-4D11-9DA3-9C63E2A09D63}">
           <x14:formula1>
             <xm:f>Referencias!$A$12:$A$13</xm:f>
           </x14:formula1>
-          <xm:sqref>C10:C108</xm:sqref>
+          <xm:sqref>C10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88BEFDC4-7CC1-4BA8-B9CF-86C377025BFC}">
+          <x14:formula1>
+            <xm:f>Referencias!$A$12:$A$14</xm:f>
+          </x14:formula1>
+          <xm:sqref>C11:C596</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -14046,10 +14089,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14103,29 +14146,40 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="60" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="60" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MP9Z+CXfAUzrDQIdUuO+hlom7NH6+9sTfqd/adNIC6OyFRyHV+BQ0+skDeBylY0Kq9e5zBn5QGI0xeD8eeor0Q==" saltValue="dIT8CS3+l3bdJdUMaSdd4Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+D5GH2NHgBw4BGfcM/CL7GensCYaLmEykHnYQK/zuJ7Zss5Fddz6jrby2LorxuVILox5SU/7CVl0bbVrAubi+w==" saltValue="igfRPjH25FC7m7g74qO6qg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A11:C11" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>